<commit_message>
commit the new code
</commit_message>
<xml_diff>
--- a/CutePressPractice/src/test/java/TestData/DataInput.xlsx
+++ b/CutePressPractice/src/test/java/TestData/DataInput.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmn7455\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmn7455\git\AutomationAssignment\CutePressPractice\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>SKU Code</t>
   </si>
@@ -62,13 +62,22 @@
     <t>All Colors</t>
   </si>
   <si>
-    <t>฿74.0</t>
-  </si>
-  <si>
     <t>10 Minutes to Clear Skin Rose Clay Mask</t>
   </si>
   <si>
     <t>฿399.00</t>
+  </si>
+  <si>
+    <t>฿279.00</t>
+  </si>
+  <si>
+    <t>฿129.00</t>
+  </si>
+  <si>
+    <t>฿79.00</t>
+  </si>
+  <si>
+    <t>฿74.00</t>
   </si>
 </sst>
 </file>
@@ -447,7 +456,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,14 +492,14 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>74533</v>
+        <v>70286</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="5">
-        <v>18</v>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -501,8 +510,8 @@
         <v>6</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="5">
-        <v>8</v>
+      <c r="D4" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -513,8 +522,8 @@
         <v>7</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="5">
-        <v>5</v>
+      <c r="D5" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -540,7 +549,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -548,11 +557,11 @@
         <v>74777</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>